<commit_message>
ndimas test promo provider
</commit_message>
<xml_diff>
--- a/assets/data/promo.xlsx
+++ b/assets/data/promo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew\flutter_application_1\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224082C8-1F90-498A-BA1E-D6B6884A66D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB0B7E9-B906-401E-80E6-5547537B0B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16944" yWindow="0" windowWidth="6096" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="276" windowWidth="16332" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -287,12 +287,6 @@
     <t>Cashback Voucher 20%</t>
   </si>
   <si>
-    <t>Max. discount 200rb\n
-Without Min. Transactions\n
-Takeaway Only\n
-Valid until 15 May 2023\n</t>
-  </si>
-  <si>
     <t>Takeaway</t>
   </si>
   <si>
@@ -306,6 +300,12 @@
   </si>
   <si>
     <t>S&amp;K</t>
+  </si>
+  <si>
+    <t>Max. discount 200rb
+Without Min. Transactions
+Takeaway Only
+Valid until 15 May 2023</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,10 +683,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1">
         <v>200000</v>
@@ -695,19 +695,19 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="J1" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L1" s="1">
         <v>15</v>

</xml_diff>

<commit_message>
ndimas orders fix type and pay
</commit_message>
<xml_diff>
--- a/assets/data/promo.xlsx
+++ b/assets/data/promo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew2\flutter_application_1\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riand\Documents\tmp\flutter_app\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40DF9C0-1A30-41C4-B5D7-9625282CE1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7D04FA-0344-4083-895F-BE61C687233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6870" yWindow="0" windowWidth="12330" windowHeight="7170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -831,22 +831,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="110.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="34.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="110.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="8.90625" style="1"/>
     <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="360" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -946,7 +946,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="348" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -996,7 +996,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>9999999</v>
+        <v>100000</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>13</v>

</xml_diff>